<commit_message>
Fixed BOM, added Gerber File export
</commit_message>
<xml_diff>
--- a/ArduinoShield/ArduinoShield_BOM.xlsx
+++ b/ArduinoShield/ArduinoShield_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Arduino\LabMonitoring\ArduinoShield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F966916C-F05B-4433-B969-99B54BCF9C41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2838AEC0-A41D-4E73-B8EE-67A07F944C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="555" windowWidth="26205" windowHeight="14910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArduinoShield" sheetId="1" r:id="rId1"/>
@@ -1101,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H21"/>
+  <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1112,7 @@
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" customWidth="1"/>
     <col min="4" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="62.42578125" customWidth="1"/>
+    <col min="6" max="6" width="78" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1550,24 +1550,6 @@
       </c>
       <c r="H18" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <f>SUM(C3:C18)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <f>C3+C6+C7+C8+C9+C10</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <f>C19-C20</f>
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Hole size for Arduino, Created Footprint for bigger hole sizes
</commit_message>
<xml_diff>
--- a/ArduinoShield/ArduinoShield_BOM.xlsx
+++ b/ArduinoShield/ArduinoShield_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Arduino\LabMonitoring\ArduinoShield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2838AEC0-A41D-4E73-B8EE-67A07F944C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B98061-1652-49F7-BCA2-22E8C2C55D2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1530" windowWidth="26205" windowHeight="14910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArduinoShield" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>Item</t>
   </si>
@@ -242,7 +242,13 @@
     <t>RR0306P-561-D</t>
   </si>
   <si>
-    <t>1x15 Socket Header, 2.54 mm Spacing, Matching a 6 mm long square pin</t>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>SSW-115-01-T-S</t>
+  </si>
+  <si>
+    <t>CONN RCPT 15POS 0.1 TIN PCB</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1110,7 @@
   <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,13 +1159,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
         <v>46</v>

</xml_diff>